<commit_message>
Update IP - EX 48 - Filtro avancado (Anexo).xlsx
</commit_message>
<xml_diff>
--- a/Materia_2-PowerBi/IP - EX 48 - Filtro avancado (Anexo).xlsx
+++ b/Materia_2-PowerBi/IP - EX 48 - Filtro avancado (Anexo).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bianc\4)DNC\Repositorio\DNC_DataScience\Materia_2-PowerBi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BD8A787-FCF5-489A-B811-473DC0E6179F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECD1336D-D674-45F2-90C6-642161B03745}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CONTEÚDO" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">EXPLICAÇÃO!$B$27:$D$39</definedName>
-    <definedName name="_xlnm.Extract" localSheetId="1">EXPLICAÇÃO!$J$32:$L$32</definedName>
+    <definedName name="_xlnm.Extract" localSheetId="1">EXPLICAÇÃO!$J$33:$L$33</definedName>
     <definedName name="_xlnm.Criteria" localSheetId="1">EXPLICAÇÃO!$J$27:$L$28</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="27">
   <si>
     <t>cor</t>
   </si>
@@ -117,9 +117,6 @@
   </si>
   <si>
     <t>Tabela de Critério</t>
-  </si>
-  <si>
-    <t>&gt;150</t>
   </si>
 </sst>
 </file>
@@ -1160,7 +1157,7 @@
   <sheetPr codeName="Plan1"/>
   <dimension ref="B1:Q13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -1338,10 +1335,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Plan2"/>
-  <dimension ref="B1:P39"/>
+  <dimension ref="B1:P42"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1354,6 +1351,7 @@
     <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.42578125" customWidth="1"/>
     <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" customWidth="1"/>
     <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1472,6 +1470,12 @@
       <c r="G10" s="29" t="s">
         <v>1</v>
       </c>
+      <c r="J10" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="K10" s="28" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
@@ -1485,6 +1489,12 @@
         <v>2</v>
       </c>
       <c r="G11" s="5"/>
+      <c r="J11" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="12" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
@@ -1494,8 +1504,16 @@
         <v>5</v>
       </c>
       <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="13" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
@@ -1507,6 +1525,12 @@
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
+      <c r="J13" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="K13" s="5" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="14" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
@@ -1518,6 +1542,12 @@
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
+      <c r="J14" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="K14" s="5" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="15" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
@@ -1526,6 +1556,12 @@
       <c r="C15" s="5" t="s">
         <v>3</v>
       </c>
+      <c r="J15" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="K15" s="5" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
@@ -1533,6 +1569,12 @@
       </c>
       <c r="C16" s="5" t="s">
         <v>5</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="K16" s="5" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
@@ -1621,7 +1663,7 @@
       <c r="J27" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="K27" s="31" t="s">
+      <c r="K27" s="30" t="s">
         <v>12</v>
       </c>
       <c r="L27" s="30" t="s">
@@ -1649,7 +1691,7 @@
       </c>
       <c r="J28" s="5"/>
       <c r="K28" s="9" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="L28" s="4" t="s">
         <v>17</v>
@@ -1708,7 +1750,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B33" s="10" t="s">
         <v>5</v>
       </c>
@@ -1718,8 +1760,26 @@
       <c r="D33" s="11">
         <v>102</v>
       </c>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F33" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="G33" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="H33" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="J33" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="K33" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="L33" s="28" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B34" s="10" t="s">
         <v>3</v>
       </c>
@@ -1729,8 +1789,26 @@
       <c r="D34" s="11">
         <v>143</v>
       </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F34" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="G34" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H34" s="11">
+        <v>100</v>
+      </c>
+      <c r="J34" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="K34" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="L34" s="11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B35" s="10" t="s">
         <v>5</v>
       </c>
@@ -1740,8 +1818,26 @@
       <c r="D35" s="11">
         <v>150</v>
       </c>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F35" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="G35" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H35" s="11">
+        <v>225</v>
+      </c>
+      <c r="J35" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="K35" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="L35" s="11">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B36" s="10" t="s">
         <v>3</v>
       </c>
@@ -1751,8 +1847,26 @@
       <c r="D36" s="11">
         <v>188</v>
       </c>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F36" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G36" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="H36" s="13">
+        <v>143</v>
+      </c>
+      <c r="J36" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="K36" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="L36" s="11">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B37" s="10" t="s">
         <v>5</v>
       </c>
@@ -1762,8 +1876,17 @@
       <c r="D37" s="11">
         <v>123</v>
       </c>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="J37" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="K37" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="L37" s="11">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B38" s="10" t="s">
         <v>5</v>
       </c>
@@ -1773,8 +1896,17 @@
       <c r="D38" s="11">
         <v>227</v>
       </c>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="J38" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="K38" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="L38" s="11">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B39" s="12" t="s">
         <v>7</v>
       </c>
@@ -1782,6 +1914,48 @@
         <v>13</v>
       </c>
       <c r="D39" s="13">
+        <v>190</v>
+      </c>
+      <c r="J39" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="K39" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="L39" s="11">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="J40" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="K40" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="L40" s="11">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="J41" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="K41" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="L41" s="11">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="J42" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="K42" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="L42" s="13">
         <v>190</v>
       </c>
     </row>

</xml_diff>